<commit_message>
adding new commands and fixed some bugs!
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -10202,6 +10202,11 @@
       <c r="C486" t="n">
         <v>890799126</v>
       </c>
+      <c r="D486" t="inlineStr">
+        <is>
+          <t>U1485@gmail.com</t>
+        </is>
+      </c>
       <c r="G486" t="inlineStr">
         <is>
           <t>F</t>

</xml_diff>

<commit_message>
adding reset_password and some Bug fixed!
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="181029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -27,7 +27,9 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <sz val="8"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -48,10 +50,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
@@ -59,9 +62,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -431,15 +436,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H503"/>
+  <dimension ref="A1:H508"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A480" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C484" sqref="C484"/>
+      <selection activeCell="D487" sqref="D487"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -9504,7 +9509,7 @@
       </c>
       <c r="H451" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>T</t>
         </is>
       </c>
     </row>
@@ -9524,7 +9529,7 @@
       </c>
       <c r="H452" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>T</t>
         </is>
       </c>
     </row>
@@ -9544,7 +9549,7 @@
       </c>
       <c r="H453" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>T</t>
         </is>
       </c>
     </row>
@@ -10196,15 +10201,17 @@
       </c>
       <c r="B486" s="2" t="inlineStr">
         <is>
-          <t>asd456#ASD</t>
-        </is>
-      </c>
-      <c r="C486" t="n">
-        <v>890799126</v>
-      </c>
-      <c r="D486" t="inlineStr">
-        <is>
-          <t>U1485@gmail.com</t>
+          <t>^gLY&amp;S!GpINztQ#r</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>Xj1BZRaz5l$AynDS</t>
+        </is>
+      </c>
+      <c r="D486" s="3" t="inlineStr">
+        <is>
+          <t>javadgraphicnet@gmail.com</t>
         </is>
       </c>
       <c r="G486" t="inlineStr">
@@ -10234,7 +10241,7 @@
       </c>
       <c r="H487" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>T</t>
         </is>
       </c>
     </row>
@@ -10274,7 +10281,7 @@
       </c>
       <c r="H489" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>T</t>
         </is>
       </c>
     </row>
@@ -10294,7 +10301,7 @@
       </c>
       <c r="H490" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>T</t>
         </is>
       </c>
     </row>
@@ -10546,7 +10553,15 @@
       </c>
     </row>
     <row r="503"/>
+    <row r="504"/>
+    <row r="505"/>
+    <row r="506"/>
+    <row r="507"/>
+    <row r="508"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D486" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>